<commit_message>
black and added region to J2 report template
</commit_message>
<xml_diff>
--- a/customized_instructions/sites_base_stations.xlsx
+++ b/customized_instructions/sites_base_stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudia/Dropbox (Indigo Wire Networks)/scripts/python/2021/devnet_create2021_no2visio/customized_instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27BDDEA-D133-5248-9DC1-A7709DBEEC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F7DCE2-CD9D-1842-83AE-151A7DBD2354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="9360" windowWidth="27640" windowHeight="16940" xr2:uid="{B2E91FC1-02B5-6F4A-9EE8-12D29A9EF996}"/>
+    <workbookView xWindow="2340" yWindow="3160" windowWidth="33540" windowHeight="10300" xr2:uid="{B2E91FC1-02B5-6F4A-9EE8-12D29A9EF996}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Site</t>
   </si>
@@ -106,6 +106,45 @@
   </si>
   <si>
     <t>BaseStationName</t>
+  </si>
+  <si>
+    <t>SFO</t>
+  </si>
+  <si>
+    <t>10.2.211.50</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>LATAM</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>APAC</t>
+  </si>
+  <si>
+    <t>EMEA</t>
+  </si>
+  <si>
+    <t>LHR</t>
+  </si>
+  <si>
+    <t>AMS</t>
+  </si>
+  <si>
+    <t>10.7.136.50</t>
+  </si>
+  <si>
+    <t>10.7.225.50</t>
+  </si>
+  <si>
+    <t>10.9.0.53</t>
+  </si>
+  <si>
+    <t>10.9.0.23</t>
   </si>
 </sst>
 </file>
@@ -457,149 +496,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE81611-F355-6548-984A-3B5A5AABF713}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="52.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="52.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="str">
         <f xml:space="preserve"> CONCATENATE(LOWER(A2),"-fwl01.uwaco.net")</f>
         <v>gdl-fwl01.uwaco.net</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <f xml:space="preserve"> CONCATENATE(LOWER(A2),"-iot-loragw01.uwaco.net")</f>
         <v>gdl-iot-loragw01.uwaco.net</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B6" si="0" xml:space="preserve"> CONCATENATE(LOWER(A3),"-fwl01.uwaco.net")</f>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C7" si="0" xml:space="preserve"> CONCATENATE(LOWER(A3),"-fwl01.uwaco.net")</f>
         <v>lax-fwl01.uwaco.net</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C6" si="1" xml:space="preserve"> CONCATENATE(LOWER(A3),"-iot-loragw01.uwaco.net")</f>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D7" si="1" xml:space="preserve"> CONCATENATE(LOWER(A3),"-iot-loragw01.uwaco.net")</f>
         <v>lax-iot-loragw01.uwaco.net</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4" si="2" xml:space="preserve"> CONCATENATE(LOWER(A4),"-fwl01.uwaco.net")</f>
+        <v>sfo-fwl01.uwaco.net</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4" si="3" xml:space="preserve"> CONCATENATE(LOWER(A4),"-iot-loragw01.uwaco.net")</f>
+        <v>sfo-iot-loragw01.uwaco.net</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>sin-fwl01.uwaco.net</v>
       </c>
-      <c r="C4" t="str">
+      <c r="D5" t="str">
         <f t="shared" si="1"/>
         <v>sin-iot-loragw01.uwaco.net</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v>ord-fwl01.uwaco.net</v>
       </c>
-      <c r="C5" t="str">
+      <c r="D6" t="str">
         <f t="shared" si="1"/>
         <v>ord-iot-loragw01.uwaco.net</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>dub-fwl01.uwaco.net</v>
       </c>
-      <c r="C6" t="str">
+      <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>dub-iot-loragw01.uwaco.net</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G7" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" ref="C8" si="4" xml:space="preserve"> CONCATENATE(LOWER(A8),"-fwl01.uwaco.net")</f>
+        <v>lhr-fwl01.uwaco.net</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" ref="D8" si="5" xml:space="preserve"> CONCATENATE(LOWER(A8),"-iot-loragw01.uwaco.net")</f>
+        <v>lhr-iot-loragw01.uwaco.net</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" ref="C9" si="6" xml:space="preserve"> CONCATENATE(LOWER(A9),"-fwl01.uwaco.net")</f>
+        <v>ams-fwl01.uwaco.net</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" ref="D9" si="7" xml:space="preserve"> CONCATENATE(LOWER(A9),"-iot-loragw01.uwaco.net")</f>
+        <v>ams-iot-loragw01.uwaco.net</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>